<commit_message>
Added transactions logging feature
Enhanced transaction readability
</commit_message>
<xml_diff>
--- a/Test Plans.xlsx
+++ b/Test Plans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Teo Sei Hau\Project\Git\AMBA3-APB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD52213F-90D3-4892-81CD-47B67BFC9B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2FE8D7-1B3F-4691-BE6B-FA6475E5ABC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="1" xr2:uid="{3DFF275C-F6BB-4F42-B6D6-D929A6041B9E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{3DFF275C-F6BB-4F42-B6D6-D929A6041B9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Stimulus" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Multiple Consecutive Write (Any) (3 - 10 txns) followed by Multiple Consecutive Read (Any) (3 - 10 txns)</t>
   </si>
   <si>
-    <t>Multiple Write (Any) (3 - 10 txns) + Multiple Read (Any) (3 - 10 txns) (Only trigger read after write)</t>
-  </si>
-  <si>
     <t>1 Write With No Wait State + 1 Read With No Wait State</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>pstate = ACCESS, pwrite = 0</t>
+  </si>
+  <si>
+    <t>Non-consecutive Multiple Write (Any) (3 - 10 txns) + Multiple Read (Any) (3 - 10 txns) (Only trigger read after write)</t>
   </si>
 </sst>
 </file>
@@ -514,15 +514,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729EC54C-6585-402F-8223-56F2D92B6FBF}">
   <dimension ref="B2:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="2"/>
     <col min="2" max="2" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="2"/>
   </cols>
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
@@ -561,7 +561,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -573,7 +573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F07F0E-2B89-4C4D-9A1C-5ED3AB1E142F}">
   <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -586,20 +586,20 @@
   <sheetData>
     <row r="2" spans="2:4" ht="21" x14ac:dyDescent="0.5">
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -607,10 +607,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -618,10 +618,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -629,10 +629,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -640,10 +640,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>